<commit_message>
Se agrega carga masiva de documentos excluidos y sector salud
</commit_message>
<xml_diff>
--- a/public/formats/co-documents-batch.xlsx
+++ b/public/formats/co-documents-batch.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="53">
   <si>
     <t>number</t>
   </si>
@@ -87,9 +87,6 @@
     <t>invoiced_quantity</t>
   </si>
   <si>
-    <t>description</t>
-  </si>
-  <si>
     <t>code</t>
   </si>
   <si>
@@ -117,9 +114,6 @@
     <t>0.00</t>
   </si>
   <si>
-    <t>PAQUETE ERC 3 A 5 Q0000395</t>
-  </si>
-  <si>
     <t>FUNDACION CLINICA NELSON MANDELA, Amor por servir</t>
   </si>
   <si>
@@ -129,9 +123,6 @@
     <t>CALLE 102 No. 24A-15</t>
   </si>
   <si>
-    <t>991500048</t>
-  </si>
-  <si>
     <t>18760000001</t>
   </si>
   <si>
@@ -139,12 +130,64 @@
   </si>
   <si>
     <t>customer</t>
+  </si>
+  <si>
+    <t>PRUEBA1</t>
+  </si>
+  <si>
+    <t>PRUEBA2</t>
+  </si>
+  <si>
+    <t>682470.00</t>
+  </si>
+  <si>
+    <t>300000.00</t>
+  </si>
+  <si>
+    <t>invoice_period_start_date</t>
+  </si>
+  <si>
+    <t>invoice_period_end_date</t>
+  </si>
+  <si>
+    <t>users_info</t>
+  </si>
+  <si>
+    <t>AF-0000500-85-XX-001,4,A89008003,OBANDO,LONDOÑO,ALEXANDER,,1,7,5,A12345;604567;AX-2345,RNA3D345;664FF04567;ARXXX-2765345,RN6645G-345;6-064XX54FF04567;XXX-2-OO-987D65345,1000-2021-0005698,1045-2FG01-0567228,3300.00,5800.00,105000.00,225000.00</t>
+  </si>
+  <si>
+    <t>AF-0000500-85-XX-001,4,A41946692,CARDONA,VILLADA,ELIZABETH,,1,7,5,A12345;604567;AX-2345,RNA3D345;664FF04567;ARXXX-2765345,RN6645G-345;6-064XX54FF04567;XXX-2-OO-987D65345,1000-2021-0005698,1045-2FG01-0567228,3300.00,5800.00,105000.00,225000.00</t>
+  </si>
+  <si>
+    <t>AF-0000500-85-XX-001,4,A89008003,OBANDO,LONDOÑO,ALEXANDER,,1,7,5,A12345;604567;AX-2345,RNA3D345;664FF04567;ARXXX-2765345,RN6645G-345;6-064XX54FF04567;XXX-2-OO-987D65345,1000-2021-0005698,1045-2FG01-0567228,3300.00,5800.00,105000.00,225000.00%AF-0000500-85-XX-001,4,A41946692,CARDONA,VILLADA,ELIZABETH,,1,7,5,A12345;604567;AX-2345,RNA3D345;664FF04567;ARXXX-2765345,RN6645G-345;6-064XX54FF04567;XXX-2-OO-987D65345,1000-2021-0005698,1045-2FG01-0567228,3300.00,5800.00,105000.00,225000.00</t>
+  </si>
+  <si>
+    <t>991500164</t>
+  </si>
+  <si>
+    <t>991500165</t>
+  </si>
+  <si>
+    <t>991500166</t>
+  </si>
+  <si>
+    <t>991500167</t>
+  </si>
+  <si>
+    <t>991500168</t>
+  </si>
+  <si>
+    <t>991500169</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="165" formatCode="[h]:mm:ss;@"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -182,10 +225,10 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -458,7 +501,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -466,18 +509,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AC2"/>
+  <dimension ref="A1:AE11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="36.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.85546875" bestFit="1" customWidth="1"/>
@@ -487,7 +530,7 @@
     <col min="11" max="11" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="17" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="21" bestFit="1" customWidth="1"/>
@@ -497,25 +540,27 @@
     <col min="21" max="21" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="17.140625" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="51.85546875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="94.7109375" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="51.85546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="94.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="24.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="24" style="3" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="244.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:31">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">
@@ -537,7 +582,7 @@
         <v>10</v>
       </c>
       <c r="K1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="L1" t="s">
         <v>11</v>
@@ -545,7 +590,7 @@
       <c r="M1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="3" t="s">
         <v>13</v>
       </c>
       <c r="O1" t="s">
@@ -588,33 +633,39 @@
         <v>25</v>
       </c>
       <c r="AB1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AC1" t="s">
         <v>5</v>
       </c>
+      <c r="AC1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>43</v>
+      </c>
     </row>
-    <row r="2" spans="1:29">
-      <c r="A2" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B2" s="1">
-        <v>45111</v>
-      </c>
-      <c r="C2" s="2">
+    <row r="2" spans="1:31">
+      <c r="A2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="3">
+        <v>45138</v>
+      </c>
+      <c r="C2" s="4">
         <v>0.69513888888888886</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>37</v>
+      <c r="D2" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="E2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H2">
         <v>3899301</v>
@@ -623,10 +674,10 @@
         <v>1006</v>
       </c>
       <c r="J2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K2">
-        <v>901021565</v>
+        <v>89008003</v>
       </c>
       <c r="L2">
         <v>1</v>
@@ -634,53 +685,896 @@
       <c r="M2">
         <v>47</v>
       </c>
-      <c r="N2" s="1">
-        <v>45142</v>
+      <c r="N2" s="3">
+        <v>45169</v>
       </c>
       <c r="O2">
         <v>30</v>
       </c>
       <c r="P2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="Q2" t="s">
+        <v>30</v>
+      </c>
+      <c r="R2" t="s">
+        <v>29</v>
+      </c>
+      <c r="S2" t="s">
+        <v>30</v>
+      </c>
+      <c r="T2" t="s">
+        <v>30</v>
+      </c>
+      <c r="U2" t="s">
+        <v>29</v>
+      </c>
+      <c r="V2">
+        <v>1</v>
+      </c>
+      <c r="W2" t="s">
+        <v>29</v>
+      </c>
+      <c r="X2" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z2" t="s">
         <v>31</v>
       </c>
-      <c r="R2" t="s">
-        <v>30</v>
-      </c>
-      <c r="S2" t="s">
+      <c r="AA2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC2" s="3">
+        <v>45108</v>
+      </c>
+      <c r="AD2" s="3">
+        <v>45138</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31">
+      <c r="A3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="3">
+        <v>45138</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0.6958333333333333</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H3">
+        <v>3899301</v>
+      </c>
+      <c r="I3">
+        <v>1006</v>
+      </c>
+      <c r="J3" t="s">
+        <v>28</v>
+      </c>
+      <c r="K3">
+        <v>89008003</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>47</v>
+      </c>
+      <c r="N3" s="3">
+        <v>45169</v>
+      </c>
+      <c r="O3">
+        <v>30</v>
+      </c>
+      <c r="P3" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>30</v>
+      </c>
+      <c r="R3" t="s">
+        <v>29</v>
+      </c>
+      <c r="S3" t="s">
+        <v>30</v>
+      </c>
+      <c r="T3" t="s">
+        <v>30</v>
+      </c>
+      <c r="U3" t="s">
+        <v>29</v>
+      </c>
+      <c r="V3">
+        <v>1</v>
+      </c>
+      <c r="W3" t="s">
+        <v>29</v>
+      </c>
+      <c r="X3" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z3" t="s">
         <v>31</v>
       </c>
-      <c r="T2" t="s">
+      <c r="AA3" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC3" s="3">
+        <v>45108</v>
+      </c>
+      <c r="AD3" s="3">
+        <v>45138</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31">
+      <c r="A4" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="3">
+        <v>45138</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0.69652777777777775</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4">
+        <v>3899301</v>
+      </c>
+      <c r="I4">
+        <v>1006</v>
+      </c>
+      <c r="J4" t="s">
+        <v>28</v>
+      </c>
+      <c r="K4">
+        <v>89008003</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <v>47</v>
+      </c>
+      <c r="N4" s="3">
+        <v>45169</v>
+      </c>
+      <c r="O4">
+        <v>30</v>
+      </c>
+      <c r="P4" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>30</v>
+      </c>
+      <c r="R4" t="s">
+        <v>29</v>
+      </c>
+      <c r="S4" t="s">
+        <v>30</v>
+      </c>
+      <c r="T4" t="s">
+        <v>30</v>
+      </c>
+      <c r="U4" t="s">
+        <v>29</v>
+      </c>
+      <c r="V4">
+        <v>1</v>
+      </c>
+      <c r="W4" t="s">
+        <v>29</v>
+      </c>
+      <c r="X4" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z4" t="s">
         <v>31</v>
       </c>
-      <c r="U2" t="s">
-        <v>30</v>
-      </c>
-      <c r="V2">
-        <v>1</v>
-      </c>
-      <c r="W2" t="s">
-        <v>30</v>
-      </c>
-      <c r="X2" t="s">
+      <c r="AA4" t="s">
         <v>32</v>
       </c>
-      <c r="Y2">
-        <v>15</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>30</v>
-      </c>
-      <c r="AA2" t="s">
+      <c r="AB4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31">
+      <c r="A5" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="3">
+        <v>45138</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0.6972222222222223</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" t="s">
         <v>33</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="H5">
+        <v>3899301</v>
+      </c>
+      <c r="I5">
+        <v>1006</v>
+      </c>
+      <c r="J5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K5">
+        <v>89008003</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <v>47</v>
+      </c>
+      <c r="N5" s="3">
+        <v>45169</v>
+      </c>
+      <c r="O5">
+        <v>30</v>
+      </c>
+      <c r="P5" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>30</v>
+      </c>
+      <c r="R5" t="s">
+        <v>29</v>
+      </c>
+      <c r="S5" t="s">
+        <v>30</v>
+      </c>
+      <c r="T5" t="s">
+        <v>30</v>
+      </c>
+      <c r="U5" t="s">
+        <v>29</v>
+      </c>
+      <c r="V5">
+        <v>1</v>
+      </c>
+      <c r="W5" t="s">
+        <v>29</v>
+      </c>
+      <c r="X5" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC5" s="3">
+        <v>45108</v>
+      </c>
+      <c r="AD5" s="3">
+        <v>45138</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31">
+      <c r="A6" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" s="3">
+        <v>45138</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0.69791666666666663</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="E6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" t="s">
         <v>27</v>
+      </c>
+      <c r="G6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6">
+        <v>3899301</v>
+      </c>
+      <c r="I6">
+        <v>1006</v>
+      </c>
+      <c r="J6" t="s">
+        <v>28</v>
+      </c>
+      <c r="K6">
+        <v>89008003</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <v>47</v>
+      </c>
+      <c r="N6" s="3">
+        <v>45169</v>
+      </c>
+      <c r="O6">
+        <v>30</v>
+      </c>
+      <c r="P6" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>30</v>
+      </c>
+      <c r="R6" t="s">
+        <v>39</v>
+      </c>
+      <c r="S6" t="s">
+        <v>30</v>
+      </c>
+      <c r="T6" t="s">
+        <v>30</v>
+      </c>
+      <c r="U6" t="s">
+        <v>39</v>
+      </c>
+      <c r="V6">
+        <v>1</v>
+      </c>
+      <c r="W6" t="s">
+        <v>29</v>
+      </c>
+      <c r="X6" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC6" s="3">
+        <v>45108</v>
+      </c>
+      <c r="AD6" s="3">
+        <v>45138</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31">
+      <c r="A7" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" s="3">
+        <v>45138</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0.69791666666666663</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H7">
+        <v>3899301</v>
+      </c>
+      <c r="I7">
+        <v>1006</v>
+      </c>
+      <c r="J7" t="s">
+        <v>28</v>
+      </c>
+      <c r="K7">
+        <v>89008003</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="M7">
+        <v>47</v>
+      </c>
+      <c r="N7" s="3">
+        <v>45169</v>
+      </c>
+      <c r="O7">
+        <v>30</v>
+      </c>
+      <c r="P7" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>30</v>
+      </c>
+      <c r="R7" t="s">
+        <v>39</v>
+      </c>
+      <c r="S7" t="s">
+        <v>30</v>
+      </c>
+      <c r="T7" t="s">
+        <v>30</v>
+      </c>
+      <c r="U7" t="s">
+        <v>39</v>
+      </c>
+      <c r="V7">
+        <v>1</v>
+      </c>
+      <c r="W7" t="s">
+        <v>29</v>
+      </c>
+      <c r="X7" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC7" s="3">
+        <v>45108</v>
+      </c>
+      <c r="AD7" s="3">
+        <v>45138</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31">
+      <c r="A8" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" s="3">
+        <v>45138</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0.69791666666666663</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H8">
+        <v>3899301</v>
+      </c>
+      <c r="I8">
+        <v>1006</v>
+      </c>
+      <c r="J8" t="s">
+        <v>28</v>
+      </c>
+      <c r="K8">
+        <v>89008003</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
+      <c r="M8">
+        <v>47</v>
+      </c>
+      <c r="N8" s="3">
+        <v>45169</v>
+      </c>
+      <c r="O8">
+        <v>30</v>
+      </c>
+      <c r="P8" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>30</v>
+      </c>
+      <c r="R8" t="s">
+        <v>39</v>
+      </c>
+      <c r="S8" t="s">
+        <v>30</v>
+      </c>
+      <c r="T8" t="s">
+        <v>30</v>
+      </c>
+      <c r="U8" t="s">
+        <v>39</v>
+      </c>
+      <c r="V8">
+        <v>1</v>
+      </c>
+      <c r="W8" t="s">
+        <v>29</v>
+      </c>
+      <c r="X8" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC8" s="3">
+        <v>45108</v>
+      </c>
+      <c r="AD8" s="3">
+        <v>45138</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31">
+      <c r="A9" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" s="3">
+        <v>45138</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0.69791666666666663</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" t="s">
+        <v>33</v>
+      </c>
+      <c r="H9">
+        <v>3899301</v>
+      </c>
+      <c r="I9">
+        <v>1006</v>
+      </c>
+      <c r="J9" t="s">
+        <v>28</v>
+      </c>
+      <c r="K9">
+        <v>89008003</v>
+      </c>
+      <c r="L9">
+        <v>1</v>
+      </c>
+      <c r="M9">
+        <v>47</v>
+      </c>
+      <c r="N9" s="3">
+        <v>45169</v>
+      </c>
+      <c r="O9">
+        <v>30</v>
+      </c>
+      <c r="P9" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>30</v>
+      </c>
+      <c r="R9" t="s">
+        <v>39</v>
+      </c>
+      <c r="S9" t="s">
+        <v>30</v>
+      </c>
+      <c r="T9" t="s">
+        <v>30</v>
+      </c>
+      <c r="U9" t="s">
+        <v>39</v>
+      </c>
+      <c r="V9">
+        <v>1</v>
+      </c>
+      <c r="W9" t="s">
+        <v>29</v>
+      </c>
+      <c r="X9" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC9" s="3">
+        <v>45108</v>
+      </c>
+      <c r="AD9" s="3">
+        <v>45138</v>
+      </c>
+      <c r="AE9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31">
+      <c r="A10" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" s="3">
+        <v>45138</v>
+      </c>
+      <c r="C10" s="4">
+        <v>0.69791666666666663</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10" t="s">
+        <v>27</v>
+      </c>
+      <c r="G10" t="s">
+        <v>33</v>
+      </c>
+      <c r="H10">
+        <v>3899301</v>
+      </c>
+      <c r="I10">
+        <v>1006</v>
+      </c>
+      <c r="J10" t="s">
+        <v>28</v>
+      </c>
+      <c r="K10">
+        <v>89008003</v>
+      </c>
+      <c r="L10">
+        <v>1</v>
+      </c>
+      <c r="M10">
+        <v>47</v>
+      </c>
+      <c r="N10" s="3">
+        <v>45169</v>
+      </c>
+      <c r="O10">
+        <v>30</v>
+      </c>
+      <c r="P10" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>30</v>
+      </c>
+      <c r="R10" t="s">
+        <v>39</v>
+      </c>
+      <c r="S10" t="s">
+        <v>30</v>
+      </c>
+      <c r="T10" t="s">
+        <v>30</v>
+      </c>
+      <c r="U10" t="s">
+        <v>39</v>
+      </c>
+      <c r="V10">
+        <v>1</v>
+      </c>
+      <c r="W10" t="s">
+        <v>29</v>
+      </c>
+      <c r="X10" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC10" s="3">
+        <v>45108</v>
+      </c>
+      <c r="AD10" s="3">
+        <v>45138</v>
+      </c>
+      <c r="AE10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31">
+      <c r="A11" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" s="3">
+        <v>45138</v>
+      </c>
+      <c r="C11" s="4">
+        <v>0.69791666666666663</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G11" t="s">
+        <v>33</v>
+      </c>
+      <c r="H11">
+        <v>3899301</v>
+      </c>
+      <c r="I11">
+        <v>1006</v>
+      </c>
+      <c r="J11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K11">
+        <v>89008003</v>
+      </c>
+      <c r="L11">
+        <v>1</v>
+      </c>
+      <c r="M11">
+        <v>47</v>
+      </c>
+      <c r="N11" s="3">
+        <v>45169</v>
+      </c>
+      <c r="O11">
+        <v>30</v>
+      </c>
+      <c r="P11" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>30</v>
+      </c>
+      <c r="R11" t="s">
+        <v>39</v>
+      </c>
+      <c r="S11" t="s">
+        <v>30</v>
+      </c>
+      <c r="T11" t="s">
+        <v>30</v>
+      </c>
+      <c r="U11" t="s">
+        <v>39</v>
+      </c>
+      <c r="V11">
+        <v>1</v>
+      </c>
+      <c r="W11" t="s">
+        <v>29</v>
+      </c>
+      <c r="X11" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC11" s="3">
+        <v>45108</v>
+      </c>
+      <c r="AD11" s="3">
+        <v>45138</v>
+      </c>
+      <c r="AE11" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>